<commit_message>
Mise à jour avec pv presque complet 09.12.2025
</commit_message>
<xml_diff>
--- a/data/electricity_producers.xlsx
+++ b/data/electricity_producers.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TM\SynergyFlex\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\TM_SynergyFlex_Nikola\SynergyFlex\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60FB215-731D-4031-BE80-6156FF916D99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280DE1AC-FC0F-4140-BBCF-0B00B4DA8D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-10740" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{79E5EDBB-6713-4204-95F5-E3E0AD6E4926}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{79E5EDBB-6713-4204-95F5-E3E0AD6E4926}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind turbine" sheetId="1" r:id="rId1"/>
     <sheet name="Photovoltaic panel" sheetId="2" r:id="rId2"/>
     <sheet name="Diesel Generator" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="23">
   <si>
     <t>Paramètres</t>
   </si>
@@ -122,12 +122,37 @@
   <si>
     <t>ans</t>
   </si>
+  <si>
+    <t xml:space="preserve">Puissance du module </t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Reviens retribution</t>
+  </si>
+  <si>
+    <t>Surface du module</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +162,14 @@
     </font>
     <font>
       <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -196,8 +229,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3361EA00-6C0B-4702-A252-07384BC13A74}" name="Tableau13" displayName="Tableau13" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10" xr:uid="{32FD8F7C-F9CD-449B-AAA7-5F71537280F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3361EA00-6C0B-4702-A252-07384BC13A74}" name="Tableau13" displayName="Tableau13" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{32FD8F7C-F9CD-449B-AAA7-5F71537280F9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AD6166D2-16B9-484B-A47B-56A09A1E594C}" name="Paramètres"/>
     <tableColumn id="2" xr3:uid="{DBC4F4B1-0539-4D5A-B44C-EF938F45DCC7}" name="Valeurs "/>
@@ -668,15 +701,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FB3C88-3D5F-43AF-B807-DE7576B8F593}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -716,75 +749,111 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>0.42</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B5">
-        <v>1800</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>1800</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>100</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>0.06</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B11">
         <v>0.05</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B12">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B10">
+      <c r="B13">
         <v>50</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>